<commit_message>
fix: the the [sic] and list supported file extensions in the instructions sheet
Signed-off-by: F.N. Claessen <felix@seita.nl>
</commit_message>
<xml_diff>
--- a/flexmeasures/ui/static/examples/sensors-data.xlsx
+++ b/flexmeasures/ui/static/examples/sensors-data.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Instructions" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -47,7 +47,7 @@
     <t xml:space="preserve">2022-12-11T10:11:00Z</t>
   </si>
   <si>
-    <t xml:space="preserve">Some requirements for the the upload file.</t>
+    <t xml:space="preserve">Some requirements for the upload file.</t>
   </si>
   <si>
     <r>
@@ -69,8 +69,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">- Excel
-- CSV
+      <t xml:space="preserve">- Excel: file extensions xlsx, xls and xlsm (or capitalized)
+- CSV: file extension csv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (or CSV)
 </t>
     </r>
     <r>
@@ -135,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -175,6 +183,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="15"/>
@@ -268,10 +281,10 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.31"/>
   </cols>
@@ -351,10 +364,10 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="43.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -445,7 +458,6 @@
       <c r="L7" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" password="c714" objects="true" scenarios="true"/>
   <mergeCells count="2">
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:L7"/>

</xml_diff>